<commit_message>
Premilinary Results With Other Solution (Starting New Branch)
</commit_message>
<xml_diff>
--- a/Synaptophysin_Image_Analysis/Lacex_summary_101119_recover_old_T1Lin19_1.xlsx
+++ b/Synaptophysin_Image_Analysis/Lacex_summary_101119_recover_old_T1Lin19_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\Synaptophysin_Image_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEB4B04-6276-424B-BC6D-4BB5B8C2B684}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C618E6BB-EC64-4930-A948-1D007886229E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{9213799F-66A2-466D-B280-AFFE4F5C011D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9213799F-66A2-466D-B280-AFFE4F5C011D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3209,16 +3209,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>20955</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>325755</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3245,16 +3245,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>44767</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>174307</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>90487</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>349567</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>20002</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3281,16 +3281,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>280987</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>6667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>90487</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>585787</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>35242</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3618,7 +3618,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="T5" sqref="T5:AB6"/>
     </sheetView>
   </sheetViews>
@@ -6741,7 +6741,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -7113,7 +7113,7 @@
         <v>43</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" ref="C13:J13" si="0">IF(NOT(ISNUMBER(FIND("E",D2))),_xlfn.CONCAT(ROUND(D2,2), " ± ", ROUND(D8,2)),_xlfn.CONCAT(LEFT(D2,4),RIGHT(D2,4), " ± ",LEFT(D8,4),RIGHT(D8,4)))</f>
+        <f t="shared" ref="D13:J13" si="0">IF(NOT(ISNUMBER(FIND("E",D2))),_xlfn.CONCAT(ROUND(D2,2), " ± ", ROUND(D8,2)),_xlfn.CONCAT(LEFT(D2,4),RIGHT(D2,4), " ± ",LEFT(D8,4),RIGHT(D8,4)))</f>
         <v>0.19 ± 0.03</v>
       </c>
       <c r="E13" t="str">

</xml_diff>